<commit_message>
Last Backend Commit, Backend Signs OFFS
</commit_message>
<xml_diff>
--- a/theory_sample/theory_endsem.xlsx
+++ b/theory_sample/theory_endsem.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raish\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CO-PO\co_po_web\theory_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85984746-A9F1-4D2B-A92A-46857F14F507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25389A6E-A453-4BDB-80D4-DED37B69E22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
   <si>
     <t>name</t>
   </si>
@@ -298,6 +298,30 @@
   </si>
   <si>
     <t>5c</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -333,12 +357,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,72 +642,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q72"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C2" s="1">
         <v>4</v>
       </c>
@@ -731,54 +757,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" t="s">
         <v>88</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -830,8 +856,11 @@
       <c r="Q4">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -883,8 +912,11 @@
       <c r="Q5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -936,8 +968,11 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -989,8 +1024,11 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1042,8 +1080,11 @@
       <c r="Q8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1095,8 +1136,11 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1148,8 +1192,11 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1201,8 +1248,11 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1254,8 +1304,11 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1307,8 +1360,11 @@
       <c r="Q13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1360,8 +1416,11 @@
       <c r="Q14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1413,8 +1472,11 @@
       <c r="Q15">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1466,8 +1528,11 @@
       <c r="Q16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1519,8 +1584,11 @@
       <c r="Q17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1572,8 +1640,11 @@
       <c r="Q18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1625,8 +1696,11 @@
       <c r="Q19">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1678,8 +1752,11 @@
       <c r="Q20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1731,8 +1808,11 @@
       <c r="Q21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1784,8 +1864,11 @@
       <c r="Q22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1837,8 +1920,11 @@
       <c r="Q23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1890,8 +1976,11 @@
       <c r="Q24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1943,8 +2032,11 @@
       <c r="Q25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1996,8 +2088,11 @@
       <c r="Q26">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2049,8 +2144,11 @@
       <c r="Q27">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2102,8 +2200,11 @@
       <c r="Q28">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2155,8 +2256,11 @@
       <c r="Q29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2208,8 +2312,11 @@
       <c r="Q30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2261,8 +2368,11 @@
       <c r="Q31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2314,8 +2424,11 @@
       <c r="Q32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2367,8 +2480,11 @@
       <c r="Q33">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2420,8 +2536,11 @@
       <c r="Q34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2473,8 +2592,11 @@
       <c r="Q35">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2526,8 +2648,11 @@
       <c r="Q36">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2579,8 +2704,11 @@
       <c r="Q37">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2632,8 +2760,11 @@
       <c r="Q38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2685,8 +2816,11 @@
       <c r="Q39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2738,8 +2872,11 @@
       <c r="Q40">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2791,8 +2928,11 @@
       <c r="Q41">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2844,8 +2984,11 @@
       <c r="Q42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2897,8 +3040,11 @@
       <c r="Q43">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2950,8 +3096,11 @@
       <c r="Q44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3003,8 +3152,11 @@
       <c r="Q45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -3056,8 +3208,11 @@
       <c r="Q46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -3109,8 +3264,11 @@
       <c r="Q47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3162,8 +3320,11 @@
       <c r="Q48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -3215,8 +3376,11 @@
       <c r="Q49">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3268,8 +3432,11 @@
       <c r="Q50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -3321,8 +3488,11 @@
       <c r="Q51">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -3374,8 +3544,11 @@
       <c r="Q52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -3427,8 +3600,11 @@
       <c r="Q53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -3480,8 +3656,11 @@
       <c r="Q54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R54" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -3533,8 +3712,11 @@
       <c r="Q55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -3586,8 +3768,11 @@
       <c r="Q56">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3639,8 +3824,11 @@
       <c r="Q57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -3692,8 +3880,11 @@
       <c r="Q58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -3745,8 +3936,11 @@
       <c r="Q59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -3798,8 +3992,11 @@
       <c r="Q60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3851,8 +4048,11 @@
       <c r="Q61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -3904,8 +4104,11 @@
       <c r="Q62">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -3957,8 +4160,11 @@
       <c r="Q63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R63" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -4010,8 +4216,11 @@
       <c r="Q64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -4063,8 +4272,11 @@
       <c r="Q65">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -4116,8 +4328,11 @@
       <c r="Q66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -4169,8 +4384,11 @@
       <c r="Q67">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -4222,8 +4440,11 @@
       <c r="Q68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -4275,8 +4496,11 @@
       <c r="Q69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R69" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -4328,8 +4552,11 @@
       <c r="Q70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R70" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -4381,8 +4608,11 @@
       <c r="Q71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -4433,6 +4663,9 @@
       </c>
       <c r="Q72">
         <v>3</v>
+      </c>
+      <c r="R72" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>